<commit_message>
Clockmode var init value changed
</commit_message>
<xml_diff>
--- a/Teile/Teileliste_2012_09_30.xlsx
+++ b/Teile/Teileliste_2012_09_30.xlsx
@@ -610,7 +610,7 @@
     <t>Polyfuse, 1.0 A</t>
   </si>
   <si>
-    <t>http://de.mouser.com/ProductDetail/Littelfuse/72R050XU/?qs=sGAEpiMZZMu7EFbsM1w0nYqj83OvMWW8AHhRQEUj9io%3d</t>
+    <t>http://de.mouser.com/ProductDetail/Littelfuse/72R090XPR/?qs=sGAEpiMZZMu7EFbsM1w0nYqj83OvMWW8gNeW78HFbUU%3d</t>
   </si>
   <si>
     <t>16Mhz</t>
@@ -1781,16 +1781,16 @@
   </sheetPr>
   <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A40" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <selection activeCell="E59" activeCellId="0" pane="topLeft" sqref="E59"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A55" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
+      <selection activeCell="D80" activeCellId="0" pane="topLeft" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.69803921568628"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.9019607843137"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8470588235294"/>
-    <col collapsed="false" hidden="false" max="8" min="4" style="0" width="11.0745098039216"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.87058823529412"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.74901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.0274509803922"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="0" width="11.156862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.93725490196078"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
@@ -3261,7 +3261,7 @@
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="74">
       <c r="A74" s="9" t="n">
         <v>2</v>
       </c>
@@ -3656,8 +3656,8 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.0745098039216"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.87058823529412"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.156862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.93725490196078"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
@@ -3713,22 +3713,21 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.44313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.0941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2627450980392"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7254901960784"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3686274509804"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6313725490196"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1764705882353"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.7921568627451"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.56470588235294"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.0823529411765"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.69803921568627"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.6980392156863"/>
-    <col collapsed="false" hidden="false" max="34" min="16" style="0" width="4.89803921568628"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="8.50980392156863"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.9921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="10.9529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.49411764705882"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2745098039216"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8470588235294"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4980392156863"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7529411764706"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.2862745098039"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.8980392156863"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.63137254901961"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.2"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.76470588235294"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.7803921568627"/>
+    <col collapsed="false" hidden="false" max="34" min="16" style="0" width="4.93725490196078"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="8.57254901960784"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.05490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1" s="13">
@@ -5256,8 +5255,8 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.87058823529412"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.93725490196078"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>